<commit_message>
Activity List - Values
</commit_message>
<xml_diff>
--- a/Documentation/MCSPROJ/Activity List.xlsx
+++ b/Documentation/MCSPROJ/Activity List.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="16925"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mlbel\Documents\3rd year\Term 2\MCSPROJ - Applied Project for IT-MI\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Project---Reservation-System\Documentation\MCSPROJ\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="40">
   <si>
     <t>Activity Name</t>
   </si>
@@ -45,16 +45,137 @@
   </si>
   <si>
     <t>Milestone</t>
+  </si>
+  <si>
+    <t>Meeting</t>
+  </si>
+  <si>
+    <t>Planning</t>
+  </si>
+  <si>
+    <t>Create Project Team</t>
+  </si>
+  <si>
+    <t>Create Project Schedule</t>
+  </si>
+  <si>
+    <t>Project Scope</t>
+  </si>
+  <si>
+    <t>Project Charter</t>
+  </si>
+  <si>
+    <t>Project Plan</t>
+  </si>
+  <si>
+    <t>Analysis</t>
+  </si>
+  <si>
+    <t>Requirements Gathering</t>
+  </si>
+  <si>
+    <t>Conduct Client Interview</t>
+  </si>
+  <si>
+    <t>Analyze Result of Interview</t>
+  </si>
+  <si>
+    <t>Analyze Client's Business 
+Process</t>
+  </si>
+  <si>
+    <t>Completion of
+Requirements</t>
+  </si>
+  <si>
+    <t>Signing of Project Adviser
+Request Form</t>
+  </si>
+  <si>
+    <t>Client Interview</t>
+  </si>
+  <si>
+    <t>Draft of Event Table, Use 
+Case Diagram, Use Case Full
+Description</t>
+  </si>
+  <si>
+    <t>Consultation with Advisers</t>
+  </si>
+  <si>
+    <t>Signing of Status Report
+Week 1</t>
+  </si>
+  <si>
+    <t>Meeting with Client</t>
+  </si>
+  <si>
+    <t>Draft of DFD/CFD/ERD/DD</t>
+  </si>
+  <si>
+    <t>Signing of Status Report
+Week 2</t>
+  </si>
+  <si>
+    <t>Input Requirements on
+Project Wiki</t>
+  </si>
+  <si>
+    <t>Draft of Activity List, WBS,
+Gantt Chart</t>
+  </si>
+  <si>
+    <t>Signing of Status Report
+Week 3</t>
+  </si>
+  <si>
+    <t>Signing of Project Panelist Form</t>
+  </si>
+  <si>
+    <t>Draft of Proposed System
+(GUI)</t>
+  </si>
+  <si>
+    <t>Finalize all requirements
+needed for documentation</t>
+  </si>
+  <si>
+    <t>Draft of Documentation</t>
+  </si>
+  <si>
+    <t>Proofread Documentation</t>
+  </si>
+  <si>
+    <t>Signing of Status Reports
+Week 4</t>
+  </si>
+  <si>
+    <t>Creating of Final Document</t>
+  </si>
+  <si>
+    <t>Defense</t>
+  </si>
+  <si>
+    <t>Submission of Fina
+Document</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -68,7 +189,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -76,23 +197,53 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Heading 3" xfId="1" builtinId="18"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="4">
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -103,6 +254,22 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A1:G33" totalsRowShown="0" headerRowDxfId="0" headerRowCellStyle="Heading 3">
+  <autoFilter ref="A1:G33"/>
+  <tableColumns count="7">
+    <tableColumn id="1" name="Activity #" dataDxfId="3"/>
+    <tableColumn id="2" name="Activity Name" dataDxfId="2"/>
+    <tableColumn id="3" name="Activity Name Description" dataDxfId="1"/>
+    <tableColumn id="4" name="# of Days"/>
+    <tableColumn id="5" name="Start Date"/>
+    <tableColumn id="6" name="Dependency"/>
+    <tableColumn id="7" name="Milestone"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -402,50 +569,408 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.625" customWidth="1"/>
-    <col min="2" max="2" width="15.625" customWidth="1"/>
-    <col min="3" max="3" width="21.625" customWidth="1"/>
-    <col min="4" max="4" width="15.625" customWidth="1"/>
-    <col min="5" max="5" width="10.625" customWidth="1"/>
-    <col min="6" max="6" width="15.5" customWidth="1"/>
-    <col min="7" max="7" width="15.625" customWidth="1"/>
+    <col min="1" max="1" width="15.85546875" customWidth="1"/>
+    <col min="2" max="2" width="18.140625" customWidth="1"/>
+    <col min="3" max="3" width="30.28515625" customWidth="1"/>
+    <col min="4" max="4" width="15.5703125" customWidth="1"/>
+    <col min="5" max="5" width="15" customWidth="1"/>
+    <col min="6" max="6" width="18.42578125" customWidth="1"/>
+    <col min="7" max="7" width="15.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
     </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C3" s="2"/>
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>8</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>9</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>10</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>11</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>12</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>13</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>14</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>15</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>16</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <v>17</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <v>18</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
+        <v>19</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
+        <v>20</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A22" s="1">
+        <v>21</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A23" s="1">
+        <v>22</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A24" s="1">
+        <v>23</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A25" s="1">
+        <v>24</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A26" s="1">
+        <v>25</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A27" s="1">
+        <v>26</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A28" s="1">
+        <v>27</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A29" s="1">
+        <v>28</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A30" s="1">
+        <v>29</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A31" s="1">
+        <v>30</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A32" s="1">
+        <v>31</v>
+      </c>
+      <c r="B32" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A33" s="1">
+        <v>32</v>
+      </c>
+      <c r="B33" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B34" s="3"/>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B35" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>